<commit_message>
updates to the files
</commit_message>
<xml_diff>
--- a/projects/PhenoRef.xlsx
+++ b/projects/PhenoRef.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cultivation\Records\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDE2C6-7A95-4059-BE00-EBA228CF6B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3898902-066A-48A5-A0C0-E1246FAAD402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="1875" windowWidth="17205" windowHeight="9900" activeTab="2" xr2:uid="{F66EE820-1DB0-4463-A333-A28DA4FAD05B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{F66EE820-1DB0-4463-A333-A28DA4FAD05B}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet.cult" sheetId="12" r:id="rId1"/>
@@ -47,20 +47,20 @@
     <definedName name="_Hlk8307326" localSheetId="11">RetiredPhenos2!$C$2</definedName>
     <definedName name="_Hlk8307373" localSheetId="4">Master!$C$16</definedName>
     <definedName name="_Hlk8307373" localSheetId="11">RetiredPhenos2!#REF!</definedName>
-    <definedName name="_xlcn.WorksheetConnection_PhenoRef.xlsxTable31" hidden="1">Table3[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_PhenoRef.xlsxTable3" hidden="1">Table3[]</definedName>
     <definedName name="Slicer_1._Phenotype">#N/A</definedName>
     <definedName name="Slicer_Round">#N/A</definedName>
     <definedName name="Slicer_Time_requirement">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="89" r:id="rId19"/>
-    <pivotCache cacheId="90" r:id="rId20"/>
+    <pivotCache cacheId="24" r:id="rId19"/>
+    <pivotCache cacheId="25" r:id="rId20"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
       <x14:pivotCaches>
-        <pivotCache cacheId="91" r:id="rId21"/>
+        <pivotCache cacheId="26" r:id="rId21"/>
       </x14:pivotCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -102,7 +102,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_PhenoRef.xlsxTable31"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_PhenoRef.xlsxTable3"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1919,9 +1919,6 @@
     <t>Spread branches slightly into the first trellis, propping them up into the second later on.</t>
   </si>
   <si>
-    <t>Trellis should be set slightly above canopy level (2-3 squares on PIPP rack).</t>
-  </si>
-  <si>
     <t>Main branches are strong, and the overall plant structure is orthotropic. While the second trellis could be skipped overall, it is useful to prevent the heavy branches from flopping late into flower. Therefore, it can be set pretty high.</t>
   </si>
   <si>
@@ -2232,6 +2229,9 @@
   </si>
   <si>
     <t>Above 35 f/sq.ft. tested flower</t>
+  </si>
+  <si>
+    <t>Trellis should be set slightly above canopy level (2-3 squares on PIPP rack). Plants should still be close enough to the trellis to be able to be trained outwards within the next week.</t>
   </si>
 </sst>
 </file>
@@ -3813,56 +3813,11 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3886,6 +3841,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3912,6 +3876,45 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3929,9 +3932,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11674,7 +11674,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2DAA20C5-C575-4C6F-8F24-B8F829045D41}" name="PivotTable5" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2DAA20C5-C575-4C6F-8F24-B8F829045D41}" name="PivotTable5" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -11796,7 +11796,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EED1AA62-6AD3-498A-9DD5-CD7C4FB88AEB}" name="PivotTable2" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EED1AA62-6AD3-498A-9DD5-CD7C4FB88AEB}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K3:AA58" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -12316,6 +12316,11 @@
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
+    </filterColumn>
+    <filterColumn colId="28">
+      <filters>
+        <filter val="Trellis should be set slightly above canopy level (2-3 squares on PIPP rack)."/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK22">
@@ -13198,7 +13203,7 @@
     </row>
     <row r="15" spans="1:19" ht="96.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="C15" s="170" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D15" s="171"/>
       <c r="E15" s="172" t="str">
@@ -13225,7 +13230,7 @@
     </row>
     <row r="18" spans="1:8" ht="96.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="C18" s="170" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D18" s="171"/>
       <c r="E18" s="172" t="str">
@@ -13291,7 +13296,7 @@
       <c r="A24" s="136"/>
       <c r="B24" s="136"/>
       <c r="C24" s="170" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D24" s="171"/>
       <c r="E24" s="178">
@@ -13305,7 +13310,7 @@
       <c r="A25" s="136"/>
       <c r="B25" s="136"/>
       <c r="C25" s="170" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D25" s="171"/>
       <c r="E25" s="179">
@@ -13328,7 +13333,7 @@
       <c r="A27" s="136"/>
       <c r="B27" s="136"/>
       <c r="C27" s="170" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D27" s="171"/>
       <c r="E27" s="174" t="str">
@@ -13386,11 +13391,11 @@
     </row>
     <row r="35" spans="1:10" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="136"/>
-      <c r="H35" s="244" t="s">
+      <c r="H35" s="245" t="s">
         <v>565</v>
       </c>
       <c r="I35" s="239" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J35" s="180" t="str">
         <f>_xlfn.CONCAT(INDEX(Table3[Pruning Requirements (Flower)],MATCH($E$8,Table3[Phenotype],0)), " prune approach")</f>
@@ -13399,9 +13404,9 @@
     </row>
     <row r="36" spans="1:10" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="136"/>
-      <c r="H36" s="244"/>
+      <c r="H36" s="245"/>
       <c r="I36" s="239" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J36" s="242" t="str">
         <f>INDEX(Table3[Pruning Technique],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13412,7 +13417,7 @@
       <c r="A37" s="136"/>
       <c r="H37" s="210"/>
       <c r="I37" s="239" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J37" s="243" t="str">
         <f>INDEX(Table3[Time requirement],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13430,11 +13435,11 @@
     </row>
     <row r="39" spans="1:10" ht="392.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="136"/>
-      <c r="H39" s="244" t="s">
+      <c r="H39" s="245" t="s">
         <v>566</v>
       </c>
       <c r="I39" s="170" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J39" s="180" t="str">
         <f>INDEX(Table3[Second and Third Trellis Instructions],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13443,9 +13448,9 @@
     </row>
     <row r="40" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="136"/>
-      <c r="H40" s="244"/>
+      <c r="H40" s="245"/>
       <c r="I40" s="170" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J40" s="206" t="str">
         <f>INDEX(Table3[Trellising Technique],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13463,11 +13468,11 @@
     </row>
     <row r="42" spans="1:10" ht="408" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="136"/>
-      <c r="H42" s="244" t="s">
+      <c r="H42" s="245" t="s">
         <v>567</v>
       </c>
       <c r="I42" s="170" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J42" s="180" t="str">
         <f>INDEX(Table3[Training Technique],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13476,9 +13481,9 @@
     </row>
     <row r="43" spans="1:10" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="136"/>
-      <c r="H43" s="244"/>
+      <c r="H43" s="245"/>
       <c r="I43" s="170" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J43" s="180" t="str">
         <f>INDEX(Table3[Recommended training times],MATCH($E$8,Table3[Phenotype],0))</f>
@@ -13630,7 +13635,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="219" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B1" s="220" t="s">
         <v>62</v>
@@ -13675,7 +13680,7 @@
         <v>10</v>
       </c>
       <c r="P1" s="220" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Q1" s="220" t="s">
         <v>7</v>
@@ -13689,55 +13694,55 @@
         <v>44183.52857638889</v>
       </c>
       <c r="B2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C2" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C2" s="215" t="s">
+      <c r="D2" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D2" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E2" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="F2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G2" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="H2" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="I2" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="F2" s="215" t="s">
+      <c r="J2" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G2" s="215" t="s">
+      <c r="K2" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="H2" s="215" t="s">
+      <c r="L2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="N2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="O2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="P2" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q2" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I2" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J2" s="215" t="s">
+      <c r="R2" s="218" t="s">
         <v>677</v>
-      </c>
-      <c r="K2" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="L2" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M2" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="N2" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="O2" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="P2" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q2" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="R2" s="218" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13745,64 +13750,64 @@
         <v>44183.532523148147</v>
       </c>
       <c r="B3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C3" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C3" s="215" t="s">
+      <c r="D3" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D3" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E3" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F3" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="H3" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="J3" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="K3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M3" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="N3" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="O3" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="H3" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I3" s="215" t="s">
+      <c r="P3" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="Q3" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="R3" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="J3" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="K3" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L3" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M3" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="N3" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="O3" s="215" t="s">
-        <v>677</v>
-      </c>
-      <c r="P3" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="Q3" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="R3" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U3" s="231" t="s">
         <v>92</v>
       </c>
       <c r="V3" s="232" t="s">
+        <v>679</v>
+      </c>
+      <c r="W3" s="233" t="s">
         <v>680</v>
-      </c>
-      <c r="W3" s="233" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13810,53 +13815,53 @@
         <v>44183.624814814815</v>
       </c>
       <c r="B4" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C4" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D4" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E4" s="215"/>
       <c r="F4" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G4" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H4" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="I4" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J4" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G4" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H4" s="215" t="s">
+      <c r="K4" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="I4" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J4" s="215" t="s">
+      <c r="L4" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K4" s="215" t="s">
+      <c r="M4" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="L4" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="M4" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="N4" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O4" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P4" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q4" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R4" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U4" s="226" t="s">
         <v>28</v>
@@ -13865,7 +13870,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="W4" s="218" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -13873,55 +13878,55 @@
         <v>44183.638020833336</v>
       </c>
       <c r="B5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C5" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C5" s="215" t="s">
+      <c r="D5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="E5" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="F5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="H5" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D5" s="215" t="s">
+      <c r="I5" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J5" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="E5" s="215" t="s">
+      <c r="K5" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="F5" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="G5" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="H5" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I5" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J5" s="215" t="s">
+      <c r="L5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="N5" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="O5" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K5" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="L5" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M5" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="N5" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="O5" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="P5" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q5" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="R5" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U5" s="226" t="s">
         <v>584</v>
@@ -13930,7 +13935,7 @@
         <v>2.06</v>
       </c>
       <c r="W5" s="218" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -13938,55 +13943,55 @@
         <v>44183.643553240741</v>
       </c>
       <c r="B6" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C6" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C6" s="215" t="s">
+      <c r="D6" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D6" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E6" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F6" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G6" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H6" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G6" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H6" s="215" t="s">
+      <c r="I6" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I6" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="J6" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="K6" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L6" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M6" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K6" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L6" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M6" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="N6" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O6" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P6" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q6" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R6" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U6" s="227" t="s">
         <v>6</v>
@@ -13995,7 +14000,7 @@
         <v>2.29</v>
       </c>
       <c r="W6" s="218" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14003,55 +14008,55 @@
         <v>44183.644224537034</v>
       </c>
       <c r="B7" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C7" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C7" s="215" t="s">
+      <c r="D7" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D7" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E7" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F7" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G7" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H7" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G7" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H7" s="215" t="s">
+      <c r="I7" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I7" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="J7" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="K7" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L7" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M7" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K7" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L7" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M7" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="N7" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O7" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P7" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q7" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R7" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U7" s="227" t="s">
         <v>469</v>
@@ -14060,7 +14065,7 @@
         <v>2.29</v>
       </c>
       <c r="W7" s="218" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14068,55 +14073,55 @@
         <v>44183.653298611112</v>
       </c>
       <c r="B8" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C8" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C8" s="215" t="s">
+      <c r="D8" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D8" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E8" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F8" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G8" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H8" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I8" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J8" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G8" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H8" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I8" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J8" s="215" t="s">
+      <c r="K8" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K8" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="L8" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M8" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="N8" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="N8" s="215" t="s">
+      <c r="O8" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="P8" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q8" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="O8" s="215" t="s">
+      <c r="R8" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="P8" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q8" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="R8" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U8" s="227" t="s">
         <v>39</v>
@@ -14125,7 +14130,7 @@
         <v>2.29</v>
       </c>
       <c r="W8" s="218" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14133,53 +14138,53 @@
         <v>44183.664548611108</v>
       </c>
       <c r="B9" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="D9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="E9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="F9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="G9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I9" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J9" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="D9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="E9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="F9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="G9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I9" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J9" s="215" t="s">
+      <c r="K9" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L9" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M9" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K9" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L9" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M9" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="N9" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O9" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P9" s="215"/>
       <c r="Q9" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="R9" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="R9" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U9" s="228" t="s">
         <v>33</v>
@@ -14188,7 +14193,7 @@
         <v>3.12</v>
       </c>
       <c r="W9" s="218" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14196,53 +14201,53 @@
         <v>44183.716539351852</v>
       </c>
       <c r="B10" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="D10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="E10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="F10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="G10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I10" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J10" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="D10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="E10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="F10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="G10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I10" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J10" s="215" t="s">
+      <c r="K10" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L10" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M10" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K10" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L10" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M10" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="N10" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="O10" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P10" s="215"/>
       <c r="Q10" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="R10" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="R10" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U10" s="228" t="s">
         <v>579</v>
@@ -14251,7 +14256,7 @@
         <v>3.24</v>
       </c>
       <c r="W10" s="218" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14259,55 +14264,55 @@
         <v>44183.836747685185</v>
       </c>
       <c r="B11" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C11" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C11" s="215" t="s">
+      <c r="D11" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D11" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="E11" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F11" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G11" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H11" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I11" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J11" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G11" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H11" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I11" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J11" s="215" t="s">
+      <c r="K11" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K11" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="L11" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M11" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="N11" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="N11" s="215" t="s">
+      <c r="O11" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="P11" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q11" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="O11" s="215" t="s">
+      <c r="R11" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="P11" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q11" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="R11" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U11" s="228" t="s">
         <v>582</v>
@@ -14316,7 +14321,7 @@
         <v>3.24</v>
       </c>
       <c r="W11" s="218" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -14324,55 +14329,55 @@
         <v>44183.85255787037</v>
       </c>
       <c r="B12" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="D12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="E12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="F12" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="H12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I12" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J12" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="D12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="E12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="F12" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="G12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I12" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J12" s="215" t="s">
+      <c r="K12" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L12" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="M12" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="N12" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K12" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L12" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="M12" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="N12" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="O12" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P12" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q12" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="R12" s="218" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="U12" s="228" t="s">
         <v>47</v>
@@ -14381,7 +14386,7 @@
         <v>3.35</v>
       </c>
       <c r="W12" s="218" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14389,55 +14394,55 @@
         <v>44183.879594907405</v>
       </c>
       <c r="B13" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C13" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C13" s="215" t="s">
+      <c r="D13" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="E13" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="F13" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G13" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D13" s="215" t="s">
+      <c r="H13" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="E13" s="215" t="s">
+      <c r="I13" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="F13" s="215" t="s">
+      <c r="J13" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G13" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H13" s="215" t="s">
+      <c r="K13" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I13" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J13" s="215" t="s">
+      <c r="L13" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K13" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="L13" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="M13" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="N13" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O13" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="P13" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q13" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R13" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U13" s="229" t="s">
         <v>7</v>
@@ -14446,7 +14451,7 @@
         <v>3.71</v>
       </c>
       <c r="W13" s="218" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14454,55 +14459,55 @@
         <v>44183.909016203703</v>
       </c>
       <c r="B14" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C14" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C14" s="215" t="s">
+      <c r="D14" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="E14" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="F14" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G14" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D14" s="215" t="s">
+      <c r="H14" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="E14" s="215" t="s">
+      <c r="I14" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="F14" s="215" t="s">
+      <c r="J14" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G14" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="H14" s="215" t="s">
+      <c r="K14" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I14" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J14" s="215" t="s">
+      <c r="L14" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K14" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="L14" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="M14" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="N14" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O14" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="P14" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q14" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R14" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U14" s="229" t="s">
         <v>25</v>
@@ -14511,7 +14516,7 @@
         <v>3.82</v>
       </c>
       <c r="W14" s="218" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14519,55 +14524,55 @@
         <v>44184.692314814813</v>
       </c>
       <c r="B15" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="C15" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="D15" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="E15" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="F15" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="G15" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="C15" s="215" t="s">
+      <c r="H15" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="D15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="E15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="F15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="G15" s="215" t="s">
+      <c r="I15" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="H15" s="215" t="s">
+      <c r="J15" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="K15" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="I15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J15" s="215" t="s">
+      <c r="L15" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="L15" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="M15" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="N15" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O15" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="P15" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q15" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="R15" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="P15" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q15" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="R15" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U15" s="229" t="s">
         <v>21</v>
@@ -14576,7 +14581,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="W15" s="218" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14584,55 +14589,55 @@
         <v>44186.3908912037</v>
       </c>
       <c r="B16" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C16" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="D16" s="215" t="s">
+        <v>676</v>
+      </c>
+      <c r="E16" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="D16" s="215" t="s">
+      <c r="F16" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="E16" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="F16" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="G16" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="H16" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I16" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J16" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="H16" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I16" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J16" s="215" t="s">
+      <c r="K16" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K16" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="L16" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M16" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="N16" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O16" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="P16" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q16" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="R16" s="218" t="s">
         <v>676</v>
-      </c>
-      <c r="P16" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="Q16" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="R16" s="218" t="s">
-        <v>677</v>
       </c>
       <c r="U16" s="230" t="s">
         <v>23</v>
@@ -14641,7 +14646,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="W16" s="218" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14649,64 +14654,64 @@
         <v>44186.448321759257</v>
       </c>
       <c r="B17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F17" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="G17" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="H17" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="I17" s="215" t="s">
+        <v>677</v>
+      </c>
+      <c r="J17" s="215" t="s">
         <v>676</v>
       </c>
-      <c r="G17" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="H17" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="I17" s="215" t="s">
-        <v>678</v>
-      </c>
-      <c r="J17" s="215" t="s">
+      <c r="K17" s="215" t="s">
+        <v>675</v>
+      </c>
+      <c r="L17" s="215" t="s">
         <v>677</v>
       </c>
-      <c r="K17" s="215" t="s">
-        <v>676</v>
-      </c>
-      <c r="L17" s="215" t="s">
-        <v>678</v>
-      </c>
       <c r="M17" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="N17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O17" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P17" s="215" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q17" s="215" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="R17" s="218" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U17" s="230" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="V17" s="225">
         <v>4.29</v>
       </c>
       <c r="W17" s="218" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14714,55 +14719,55 @@
         <v>44186.478692129633</v>
       </c>
       <c r="B18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="C18" s="223" t="s">
+        <v>677</v>
+      </c>
+      <c r="D18" s="223" t="s">
+        <v>677</v>
+      </c>
+      <c r="E18" s="223" t="s">
         <v>676</v>
       </c>
-      <c r="C18" s="223" t="s">
-        <v>678</v>
-      </c>
-      <c r="D18" s="223" t="s">
-        <v>678</v>
-      </c>
-      <c r="E18" s="223" t="s">
+      <c r="F18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="G18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="H18" s="223" t="s">
+        <v>676</v>
+      </c>
+      <c r="I18" s="223" t="s">
         <v>677</v>
       </c>
-      <c r="F18" s="223" t="s">
+      <c r="J18" s="223" t="s">
         <v>676</v>
       </c>
-      <c r="G18" s="223" t="s">
-        <v>676</v>
-      </c>
-      <c r="H18" s="223" t="s">
+      <c r="K18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="L18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="M18" s="223" t="s">
+        <v>675</v>
+      </c>
+      <c r="N18" s="223" t="s">
         <v>677</v>
       </c>
-      <c r="I18" s="223" t="s">
-        <v>678</v>
-      </c>
-      <c r="J18" s="223" t="s">
+      <c r="O18" s="223" t="s">
         <v>677</v>
       </c>
-      <c r="K18" s="223" t="s">
-        <v>676</v>
-      </c>
-      <c r="L18" s="223" t="s">
-        <v>676</v>
-      </c>
-      <c r="M18" s="223" t="s">
-        <v>676</v>
-      </c>
-      <c r="N18" s="223" t="s">
-        <v>678</v>
-      </c>
-      <c r="O18" s="223" t="s">
-        <v>678</v>
-      </c>
       <c r="P18" s="223" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q18" s="223" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="R18" s="224" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="U18" s="230" t="s">
         <v>10</v>
@@ -14771,7 +14776,7 @@
         <v>4.29</v>
       </c>
       <c r="W18" s="218" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14782,12 +14787,12 @@
         <v>4.41</v>
       </c>
       <c r="W19" s="218" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
@@ -14832,7 +14837,7 @@
         <v>10</v>
       </c>
       <c r="P20" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Q20" t="s">
         <v>7</v>
@@ -14847,7 +14852,7 @@
         <v>4.76</v>
       </c>
       <c r="W20" s="224" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -15804,7 +15809,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B38">
         <f>SUBTOTAL(101,Table16[92CK119])</f>
@@ -15898,61 +15903,61 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="282" t="s">
-        <v>688</v>
-      </c>
-      <c r="D1" s="282"/>
-      <c r="E1" s="282"/>
+      <c r="C1" s="283" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1" s="283"/>
+      <c r="E1" s="283"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="236" t="s">
+        <v>670</v>
+      </c>
+      <c r="D2" s="237" t="s">
         <v>671</v>
       </c>
-      <c r="D2" s="237" t="s">
+      <c r="E2" s="238" t="s">
         <v>672</v>
-      </c>
-      <c r="E2" s="238" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="236" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B3" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="237" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B4" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="236" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B5" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="236" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B6" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="236" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B7" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -15960,103 +15965,103 @@
         <v>429</v>
       </c>
       <c r="B8" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="237" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B9" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="238" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B10" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="238" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B11" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="236" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B12" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="237" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B13" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="238" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B14" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="238" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B15" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="238" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B16" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="238" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B17" s="238" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="237" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B18" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="237" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B19" s="237" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="236" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B20" s="236" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -30161,15 +30166,15 @@
     <row r="6" spans="1:19" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
-      <c r="C6" s="248" t="s">
+      <c r="C6" s="268" t="s">
         <v>364</v>
       </c>
-      <c r="D6" s="249" t="str">
+      <c r="D6" s="269" t="str">
         <f>INDEX(Table3[Phenotype],C5,0)</f>
         <v>92CK119</v>
       </c>
-      <c r="E6" s="249"/>
-      <c r="F6" s="249"/>
+      <c r="E6" s="269"/>
+      <c r="F6" s="269"/>
       <c r="G6" s="81"/>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
@@ -30185,10 +30190,10 @@
     <row r="7" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
-      <c r="C7" s="248"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="269"/>
+      <c r="E7" s="269"/>
+      <c r="F7" s="269"/>
       <c r="G7" s="81"/>
       <c r="H7" s="116" t="s">
         <v>388</v>
@@ -30199,7 +30204,7 @@
       </c>
       <c r="J7" s="117">
         <f ca="1">TODAY()</f>
-        <v>44188</v>
+        <v>44195</v>
       </c>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
@@ -30212,10 +30217,10 @@
     <row r="8" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
-      <c r="C8" s="248"/>
-      <c r="D8" s="249"/>
-      <c r="E8" s="249"/>
-      <c r="F8" s="249"/>
+      <c r="C8" s="268"/>
+      <c r="D8" s="269"/>
+      <c r="E8" s="269"/>
+      <c r="F8" s="269"/>
       <c r="G8" s="81"/>
       <c r="H8" s="119" t="s">
         <v>394</v>
@@ -30236,25 +30241,25 @@
       <c r="C9" s="105" t="s">
         <v>338</v>
       </c>
-      <c r="D9" s="250" t="e">
+      <c r="D9" s="270" t="e">
         <f>INDEX(#REF!,MATCH($D$6,Table3[Phenotype],0))</f>
         <v>#REF!</v>
       </c>
-      <c r="E9" s="250"/>
-      <c r="F9" s="250"/>
+      <c r="E9" s="270"/>
+      <c r="F9" s="270"/>
       <c r="G9" s="79"/>
       <c r="H9" s="112" t="s">
         <v>351</v>
       </c>
-      <c r="I9" s="251" t="str">
+      <c r="I9" s="254" t="str">
         <f>INDEX(Table3[Pruning Requirements (Veg)],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>not determined</v>
       </c>
-      <c r="J9" s="252"/>
-      <c r="K9" s="252"/>
-      <c r="L9" s="252"/>
-      <c r="M9" s="252"/>
-      <c r="N9" s="253"/>
+      <c r="J9" s="255"/>
+      <c r="K9" s="255"/>
+      <c r="L9" s="255"/>
+      <c r="M9" s="255"/>
+      <c r="N9" s="256"/>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
       <c r="S9" s="34"/>
@@ -30272,11 +30277,11 @@
       <c r="H10" s="112" t="s">
         <v>352</v>
       </c>
-      <c r="I10" s="254" t="str">
+      <c r="I10" s="271" t="str">
         <f>INDEX(Table3[Pruning Requirements (Flower)],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Moderate/Heavy</v>
       </c>
-      <c r="J10" s="255"/>
+      <c r="J10" s="272"/>
       <c r="K10" s="101"/>
       <c r="L10" s="101"/>
       <c r="M10" s="101"/>
@@ -30298,18 +30303,18 @@
       </c>
       <c r="F11" s="87"/>
       <c r="G11" s="79"/>
-      <c r="H11" s="256" t="s">
+      <c r="H11" s="273" t="s">
         <v>342</v>
       </c>
-      <c r="I11" s="258" t="str">
+      <c r="I11" s="275" t="str">
         <f>INDEX(Table3[Pruning Technique],MATCH($D$6,Table3[Phenotype],0))</f>
         <v xml:space="preserve">Prune more heavily due to their potential for future growth and dense inner canopy. </v>
       </c>
-      <c r="J11" s="258"/>
-      <c r="K11" s="258"/>
-      <c r="L11" s="258"/>
-      <c r="M11" s="258"/>
-      <c r="N11" s="258"/>
+      <c r="J11" s="275"/>
+      <c r="K11" s="275"/>
+      <c r="L11" s="275"/>
+      <c r="M11" s="275"/>
+      <c r="N11" s="275"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
       <c r="S11" s="34"/>
@@ -30327,13 +30332,13 @@
       </c>
       <c r="F12" s="88"/>
       <c r="G12" s="77"/>
-      <c r="H12" s="256"/>
-      <c r="I12" s="259"/>
-      <c r="J12" s="259"/>
-      <c r="K12" s="259"/>
-      <c r="L12" s="259"/>
-      <c r="M12" s="259"/>
-      <c r="N12" s="259"/>
+      <c r="H12" s="273"/>
+      <c r="I12" s="276"/>
+      <c r="J12" s="276"/>
+      <c r="K12" s="276"/>
+      <c r="L12" s="276"/>
+      <c r="M12" s="276"/>
+      <c r="N12" s="276"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
       <c r="S12" s="34"/>
@@ -30348,13 +30353,13 @@
       <c r="E13" s="82"/>
       <c r="F13" s="79"/>
       <c r="G13" s="79"/>
-      <c r="H13" s="256"/>
-      <c r="I13" s="259"/>
-      <c r="J13" s="259"/>
-      <c r="K13" s="259"/>
-      <c r="L13" s="259"/>
-      <c r="M13" s="259"/>
-      <c r="N13" s="259"/>
+      <c r="H13" s="273"/>
+      <c r="I13" s="276"/>
+      <c r="J13" s="276"/>
+      <c r="K13" s="276"/>
+      <c r="L13" s="276"/>
+      <c r="M13" s="276"/>
+      <c r="N13" s="276"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
       <c r="S13" s="34"/>
@@ -30432,15 +30437,15 @@
       <c r="H16" s="114" t="s">
         <v>344</v>
       </c>
-      <c r="I16" s="257" t="str">
+      <c r="I16" s="274" t="str">
         <f>INDEX(Table3[Second and Third Trellis Instructions],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>set second trellis at slightly more than a hands length above the first, and add third trellis just above the canopy.</v>
       </c>
-      <c r="J16" s="257"/>
-      <c r="K16" s="257"/>
-      <c r="L16" s="257"/>
-      <c r="M16" s="257"/>
-      <c r="N16" s="257"/>
+      <c r="J16" s="274"/>
+      <c r="K16" s="274"/>
+      <c r="L16" s="274"/>
+      <c r="M16" s="274"/>
+      <c r="N16" s="274"/>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
@@ -30465,11 +30470,11 @@
       <c r="H17" s="113" t="s">
         <v>402</v>
       </c>
-      <c r="I17" s="245" t="str">
+      <c r="I17" s="265" t="str">
         <f>INDEX(Table3[Early Second],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>yes</v>
       </c>
-      <c r="J17" s="246"/>
+      <c r="J17" s="266"/>
       <c r="K17" s="123"/>
       <c r="L17" s="123"/>
       <c r="M17" s="123"/>
@@ -30490,18 +30495,18 @@
       <c r="E18" s="82"/>
       <c r="F18" s="82"/>
       <c r="G18" s="77"/>
-      <c r="H18" s="261" t="s">
+      <c r="H18" s="246" t="s">
         <v>345</v>
       </c>
-      <c r="I18" s="263" t="str">
+      <c r="I18" s="248" t="str">
         <f>INDEX(Table3[Trellising Technique],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Set second trellis very low, at about hand away from the first trellis. The third trellis can be set just above the canopy so that only tall branches poke through.</v>
       </c>
-      <c r="J18" s="264"/>
-      <c r="K18" s="264"/>
-      <c r="L18" s="264"/>
-      <c r="M18" s="264"/>
-      <c r="N18" s="265"/>
+      <c r="J18" s="249"/>
+      <c r="K18" s="249"/>
+      <c r="L18" s="249"/>
+      <c r="M18" s="249"/>
+      <c r="N18" s="250"/>
       <c r="O18" s="34"/>
       <c r="P18" s="34"/>
     </row>
@@ -30511,20 +30516,20 @@
       <c r="C19" s="110" t="s">
         <v>339</v>
       </c>
-      <c r="D19" s="254" t="str">
+      <c r="D19" s="271" t="str">
         <f>INDEX(Table3[Growth Habit],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Orthotropic</v>
       </c>
-      <c r="E19" s="255"/>
-      <c r="F19" s="260"/>
+      <c r="E19" s="272"/>
+      <c r="F19" s="277"/>
       <c r="G19" s="77"/>
-      <c r="H19" s="262"/>
-      <c r="I19" s="266"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="267"/>
-      <c r="M19" s="267"/>
-      <c r="N19" s="268"/>
+      <c r="H19" s="247"/>
+      <c r="I19" s="251"/>
+      <c r="J19" s="252"/>
+      <c r="K19" s="252"/>
+      <c r="L19" s="252"/>
+      <c r="M19" s="252"/>
+      <c r="N19" s="253"/>
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
     </row>
@@ -30534,12 +30539,12 @@
       <c r="C20" s="110" t="s">
         <v>340</v>
       </c>
-      <c r="D20" s="254" t="str">
+      <c r="D20" s="271" t="str">
         <f>INDEX(Table3[Stem Structure],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Weak</v>
       </c>
-      <c r="E20" s="255"/>
-      <c r="F20" s="260"/>
+      <c r="E20" s="272"/>
+      <c r="F20" s="277"/>
       <c r="G20" s="75"/>
       <c r="H20" s="118" t="s">
         <v>396</v>
@@ -30559,25 +30564,25 @@
       <c r="C21" s="110" t="s">
         <v>350</v>
       </c>
-      <c r="D21" s="254" t="str">
+      <c r="D21" s="271" t="str">
         <f>INDEX(Table3[Tertiary Branch Length],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>long</v>
       </c>
-      <c r="E21" s="255"/>
-      <c r="F21" s="260"/>
+      <c r="E21" s="272"/>
+      <c r="F21" s="277"/>
       <c r="G21" s="75"/>
       <c r="H21" s="125" t="s">
         <v>346</v>
       </c>
-      <c r="I21" s="251" t="str">
+      <c r="I21" s="254" t="str">
         <f>INDEX(Table3[Training Technique],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Spread into first trellis but focus on setting them on a vertical path into the second and third trellis. During or after hard prune, set and stretch tertiary branches into second and third trellis where possible.</v>
       </c>
-      <c r="J21" s="252"/>
-      <c r="K21" s="252"/>
-      <c r="L21" s="252"/>
-      <c r="M21" s="252"/>
-      <c r="N21" s="253"/>
+      <c r="J21" s="255"/>
+      <c r="K21" s="255"/>
+      <c r="L21" s="255"/>
+      <c r="M21" s="255"/>
+      <c r="N21" s="256"/>
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
     </row>
@@ -30589,18 +30594,18 @@
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
       <c r="G22" s="75"/>
-      <c r="H22" s="269" t="s">
+      <c r="H22" s="257" t="s">
         <v>353</v>
       </c>
-      <c r="I22" s="271" t="str">
+      <c r="I22" s="259" t="str">
         <f>INDEX(Table3[Recommended training times],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Week 1, Week 3, Week 6</v>
       </c>
-      <c r="J22" s="272"/>
-      <c r="K22" s="272"/>
-      <c r="L22" s="272"/>
-      <c r="M22" s="272"/>
-      <c r="N22" s="273"/>
+      <c r="J22" s="260"/>
+      <c r="K22" s="260"/>
+      <c r="L22" s="260"/>
+      <c r="M22" s="260"/>
+      <c r="N22" s="261"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
     </row>
@@ -30614,13 +30619,13 @@
       <c r="E23" s="82"/>
       <c r="F23" s="82"/>
       <c r="G23" s="77"/>
-      <c r="H23" s="270"/>
-      <c r="I23" s="274"/>
-      <c r="J23" s="275"/>
-      <c r="K23" s="275"/>
-      <c r="L23" s="275"/>
-      <c r="M23" s="275"/>
-      <c r="N23" s="276"/>
+      <c r="H23" s="258"/>
+      <c r="I23" s="262"/>
+      <c r="J23" s="263"/>
+      <c r="K23" s="263"/>
+      <c r="L23" s="263"/>
+      <c r="M23" s="263"/>
+      <c r="N23" s="264"/>
       <c r="O23" s="34"/>
       <c r="P23" s="34"/>
     </row>
@@ -30630,12 +30635,12 @@
       <c r="C24" s="111" t="s">
         <v>356</v>
       </c>
-      <c r="D24" s="250" t="str">
+      <c r="D24" s="270" t="str">
         <f>INDEX(Table3[Early/Late First Top],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>Early</v>
       </c>
-      <c r="E24" s="250"/>
-      <c r="F24" s="250"/>
+      <c r="E24" s="270"/>
+      <c r="F24" s="270"/>
       <c r="G24" s="75"/>
       <c r="H24" s="118" t="s">
         <v>397</v>
@@ -30655,12 +30660,12 @@
       <c r="C25" s="111" t="s">
         <v>341</v>
       </c>
-      <c r="D25" s="250" t="str">
+      <c r="D25" s="270" t="str">
         <f>INDEX(Table3[Topping Strategy],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>not determined</v>
       </c>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
+      <c r="E25" s="270"/>
+      <c r="F25" s="270"/>
       <c r="G25" s="80"/>
       <c r="H25" s="115" t="s">
         <v>354</v>
@@ -30688,11 +30693,11 @@
       <c r="H26" s="115" t="s">
         <v>347</v>
       </c>
-      <c r="I26" s="245">
+      <c r="I26" s="265">
         <f>INDEX(Table3[PM INDEX],MATCH($D$6,Table3[Phenotype],0))</f>
         <v>11</v>
       </c>
-      <c r="J26" s="246"/>
+      <c r="J26" s="266"/>
       <c r="K26" s="99" t="s">
         <v>398</v>
       </c>
@@ -30700,10 +30705,10 @@
         <f>(MAX(Table3[PM INDEX]))</f>
         <v>14</v>
       </c>
-      <c r="M26" s="246" t="s">
+      <c r="M26" s="266" t="s">
         <v>399</v>
       </c>
-      <c r="N26" s="247"/>
+      <c r="N26" s="267"/>
       <c r="O26" s="34"/>
       <c r="P26" s="34"/>
     </row>
@@ -30826,11 +30831,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:N19"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:N23"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="I17:J17"/>
@@ -30847,6 +30847,11 @@
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:N19"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:N23"/>
   </mergeCells>
   <conditionalFormatting sqref="I26">
     <cfRule type="cellIs" dxfId="232" priority="1" operator="greaterThan">
@@ -30921,7 +30926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9603E7ED-7A90-4A4F-ACBB-3D83EF0B66EF}">
   <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="33" zoomScaleNormal="70" zoomScaleSheetLayoutView="46" zoomScalePageLayoutView="29" workbookViewId="0">
+    <sheetView zoomScale="33" zoomScaleNormal="70" zoomScaleSheetLayoutView="46" zoomScalePageLayoutView="29" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -31008,7 +31013,7 @@
       <c r="B8" s="139" t="s">
         <v>533</v>
       </c>
-      <c r="C8" s="283" t="str">
+      <c r="C8" s="244" t="str">
         <f>INDEX(Table3[Phenotype],C5,0)</f>
         <v>SUNL006</v>
       </c>
@@ -31017,7 +31022,7 @@
     </row>
     <row r="10" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="170" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C10" s="183" t="str">
         <f>INDEX(Table3[Lineage],MATCH(C8,Table3[Phenotype],0))</f>
@@ -31027,7 +31032,7 @@
     </row>
     <row r="11" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="170" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C11" s="172" t="str">
         <f>INDEX(Table3[Classification],MATCH(C8,Table3[Phenotype],0))</f>
@@ -31042,7 +31047,7 @@
     </row>
     <row r="13" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="170" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C13" s="172" t="str">
         <f>INDEX(Table3[Dry Time],MATCH(C8,Table3[Phenotype],0))</f>
@@ -31052,7 +31057,7 @@
     </row>
     <row r="14" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="170" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C14" s="172" t="str">
         <f>INDEX(Table3[Yield Category],MATCH(C8,Table3[Phenotype],0))</f>
@@ -31062,7 +31067,7 @@
     </row>
     <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="207" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C15" s="208" t="str">
         <f>_xlfn.CONCAT((_xlfn.NUMBERVALUE(INDEX(Table3[Average THC Potency],MATCH(C8,Table3[Phenotype],0)))*100),"%)")</f>
@@ -31211,19 +31216,19 @@
     </row>
     <row r="4" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C4" t="s">
         <v>682</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>683</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>684</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>685</v>
-      </c>
-      <c r="F4" t="s">
-        <v>686</v>
       </c>
       <c r="T4" s="185" t="s">
         <v>339</v>
@@ -31246,22 +31251,22 @@
     </row>
     <row r="5" spans="1:27" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>690</v>
+      </c>
+      <c r="B5" s="155" t="s">
+        <v>694</v>
+      </c>
+      <c r="C5" s="155" t="s">
+        <v>695</v>
+      </c>
+      <c r="D5" s="155" t="s">
         <v>691</v>
       </c>
-      <c r="B5" s="155" t="s">
-        <v>695</v>
-      </c>
-      <c r="C5" s="155" t="s">
-        <v>696</v>
-      </c>
-      <c r="D5" s="155" t="s">
+      <c r="E5" s="155" t="s">
         <v>692</v>
       </c>
-      <c r="E5" s="155" t="s">
+      <c r="F5" s="155" t="s">
         <v>693</v>
-      </c>
-      <c r="F5" s="155" t="s">
-        <v>694</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -31499,11 +31504,11 @@
     </row>
     <row r="24" spans="20:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T24" s="188" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="U24" s="201"/>
       <c r="V24" s="201" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="W24" s="201"/>
       <c r="X24" s="201"/>
@@ -31589,11 +31594,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31614,6 +31619,7 @@
     <col min="24" max="24" width="17.28515625" customWidth="1"/>
     <col min="25" max="25" width="29" customWidth="1"/>
     <col min="26" max="26" width="21.140625" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" customWidth="1"/>
     <col min="28" max="28" width="19.28515625" customWidth="1"/>
     <col min="29" max="29" width="12.42578125" customWidth="1"/>
     <col min="30" max="33" width="18.28515625" customWidth="1"/>
@@ -31633,28 +31639,28 @@
         <v>405</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>408</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>348</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>349</v>
@@ -31675,7 +31681,7 @@
         <v>560</v>
       </c>
       <c r="S1" s="151" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T1" s="151" t="s">
         <v>564</v>
@@ -31732,7 +31738,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="126" t="s">
         <v>62</v>
       </c>
@@ -31759,7 +31765,7 @@
         <v>Below 30 g/sq.ft tested flower</v>
       </c>
       <c r="I2" s="126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J2" s="18">
         <v>22.083769633507853</v>
@@ -31846,7 +31852,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="127" t="s">
         <v>584</v>
       </c>
@@ -31871,7 +31877,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I3" s="127" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J3" s="18">
         <v>22.917721518987342</v>
@@ -31975,7 +31981,7 @@
         <v>0.223</v>
       </c>
       <c r="F4" s="211" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G4" s="157" t="s">
         <v>521</v>
@@ -31985,7 +31991,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I4" s="157" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J4" s="159">
         <v>16.618421052631579</v>
@@ -32046,7 +32052,7 @@
         <v>401</v>
       </c>
       <c r="AC4" s="162" t="s">
-        <v>602</v>
+        <v>706</v>
       </c>
       <c r="AD4" s="163" t="s">
         <v>198</v>
@@ -32072,7 +32078,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="126" t="s">
         <v>469</v>
       </c>
@@ -32099,7 +32105,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I5" s="126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J5" s="18">
         <v>20.464285714285715</v>
@@ -32186,7 +32192,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="126" t="s">
         <v>572</v>
       </c>
@@ -32194,7 +32200,7 @@
         <v>573</v>
       </c>
       <c r="C6" s="212" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D6" s="126" t="s">
         <v>428</v>
@@ -32209,7 +32215,7 @@
         <v>Around 30 g/sq.ft. tested flower</v>
       </c>
       <c r="I6" s="126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J6" s="18">
         <v>12.916666666666666</v>
@@ -32307,7 +32313,7 @@
         <v>Above 35 f/sq.ft. tested flower</v>
       </c>
       <c r="I7" s="126" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J7" s="18">
         <v>16.116504854368934</v>
@@ -32367,8 +32373,8 @@
       <c r="AB7" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="AC7" s="2" t="s">
-        <v>602</v>
+      <c r="AC7" s="27" t="s">
+        <v>706</v>
       </c>
       <c r="AD7" s="21" t="s">
         <v>198</v>
@@ -32394,7 +32400,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="126" t="s">
         <v>39</v>
       </c>
@@ -32421,7 +32427,7 @@
         <v>Below 30 g/sq.ft tested flower</v>
       </c>
       <c r="I8" s="126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J8" s="18">
         <v>15.808510638297872</v>
@@ -32508,7 +32514,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="126" t="s">
         <v>33</v>
       </c>
@@ -32535,7 +32541,7 @@
         <v>30-35 g/sq.ft. tested flower</v>
       </c>
       <c r="I9" s="126" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J9" s="18">
         <v>24.438848920863311</v>
@@ -32622,7 +32628,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="126" t="s">
         <v>28</v>
       </c>
@@ -32649,7 +32655,7 @@
         <v>Around 30 g/sq.ft. tested flower</v>
       </c>
       <c r="I10" s="126" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J10" s="18">
         <v>23.964285714285715</v>
@@ -32736,7 +32742,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="127" t="s">
         <v>25</v>
       </c>
@@ -32763,7 +32769,7 @@
         <v>Below 30 g/sq.ft tested flower</v>
       </c>
       <c r="I11" s="126" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J11" s="19">
         <v>21.702970297029704</v>
@@ -32850,7 +32856,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="126" t="s">
         <v>23</v>
       </c>
@@ -32877,7 +32883,7 @@
         <v>Around 30 g/sq.ft. tested flower</v>
       </c>
       <c r="I12" s="126" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J12" s="18">
         <v>24.285714285714285</v>
@@ -32964,7 +32970,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="126" t="s">
         <v>569</v>
       </c>
@@ -32972,7 +32978,7 @@
         <v>587</v>
       </c>
       <c r="C13" s="211" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D13" s="126" t="s">
         <v>428</v>
@@ -32987,7 +32993,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I13" s="126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J13" s="18">
         <v>21.528571428571428</v>
@@ -33034,7 +33040,7 @@
         <v>594</v>
       </c>
       <c r="Z13" s="17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="AA13" s="2">
         <v>2</v>
@@ -33049,7 +33055,7 @@
         <v>179</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>597</v>
@@ -33067,7 +33073,7 @@
       </c>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="127" t="s">
         <v>21</v>
       </c>
@@ -33094,7 +33100,7 @@
         <v>Above 35 f/sq.ft. tested flower</v>
       </c>
       <c r="I14" s="126" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J14" s="18">
         <v>17.078125</v>
@@ -33170,7 +33176,7 @@
         <v>325</v>
       </c>
       <c r="AH14" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AI14" s="28"/>
       <c r="AJ14" s="28">
@@ -33181,7 +33187,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="126" t="s">
         <v>582</v>
       </c>
@@ -33208,7 +33214,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I15" s="126" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J15" s="18">
         <v>14.84297520661157</v>
@@ -33295,12 +33301,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="157" t="s">
+        <v>621</v>
+      </c>
+      <c r="B16" s="157" t="s">
         <v>622</v>
-      </c>
-      <c r="B16" s="157" t="s">
-        <v>623</v>
       </c>
       <c r="C16" s="157" t="s">
         <v>457</v>
@@ -33322,7 +33328,7 @@
         <v>not yet determined</v>
       </c>
       <c r="I16" s="157" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J16" s="159">
         <v>17.886029411764707</v>
@@ -33398,7 +33404,7 @@
         <v>324</v>
       </c>
       <c r="AH16" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AI16" s="164"/>
       <c r="AJ16" s="164" t="str">
@@ -33409,7 +33415,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="127" t="s">
         <v>10</v>
       </c>
@@ -33436,7 +33442,7 @@
         <v>Around 30 g/sq.ft. tested flower</v>
       </c>
       <c r="I17" s="126" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J17" s="18">
         <v>15.651162790697674</v>
@@ -33512,7 +33518,7 @@
         <v>325</v>
       </c>
       <c r="AH17" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AI17" s="28"/>
       <c r="AJ17" s="28">
@@ -33777,7 +33783,7 @@
       </c>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="129" t="s">
         <v>7</v>
       </c>
@@ -33794,7 +33800,7 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="F21" s="129" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G21" s="129" t="s">
         <v>532</v>
@@ -33804,7 +33810,7 @@
         <v>Below 30 g/sq.ft tested flower</v>
       </c>
       <c r="I21" s="129" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J21" s="18">
         <v>22.372093023255815</v>
@@ -33891,7 +33897,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="126" t="s">
         <v>6</v>
       </c>
@@ -33918,7 +33924,7 @@
         <v>Below 30 g/sq.ft tested flower</v>
       </c>
       <c r="I22" s="126" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J22" s="18">
         <v>17.956896551724139</v>
@@ -34207,7 +34213,7 @@
     </row>
     <row r="26" spans="1:37" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="126" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B26" s="126"/>
       <c r="C26" s="126"/>
@@ -34254,7 +34260,7 @@
         <v>80</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Z26" s="17" t="str">
         <f>_xlfn.IFNA(INDEX(Table17[Category],MATCH(Table3[[#This Row],[Phenotype]],Table17[Pheno],0)),"")</f>
@@ -34273,7 +34279,7 @@
         <v>180</v>
       </c>
       <c r="AE26" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AF26" s="1" t="s">
         <v>601</v>
@@ -36279,21 +36285,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="278" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="D1" s="281" t="s">
+      <c r="B1" s="279"/>
+      <c r="D1" s="282" t="s">
         <v>283</v>
       </c>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="279">
+      <c r="A2" s="280">
         <v>44174</v>
       </c>
-      <c r="B2" s="280"/>
+      <c r="B2" s="281"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -36946,201 +36952,201 @@
   <sheetData>
     <row r="1" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="241" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B2" s="213">
         <v>16.408639172335601</v>
       </c>
       <c r="C2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="241" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B3" s="213">
         <v>27.424622059184422</v>
       </c>
       <c r="C3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="241" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B4" s="213">
         <v>27.537014329805995</v>
       </c>
       <c r="C4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="241" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B5" s="213">
         <v>27.599372894340132</v>
       </c>
       <c r="C5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="241" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B6" s="213">
         <v>27.781483718011724</v>
       </c>
       <c r="C6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="241" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B7" s="213">
         <v>28.038766469416821</v>
       </c>
       <c r="C7" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="241" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B8" s="213">
         <v>28.280751212522045</v>
       </c>
       <c r="C8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="241" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B9" s="213">
         <v>29.02890886648979</v>
       </c>
       <c r="C9" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="241" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B10" s="213">
         <v>29.630727402998239</v>
       </c>
       <c r="C10" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="241" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B11" s="213">
         <v>30.120475709754061</v>
       </c>
       <c r="C11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="241" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B12" s="213">
         <v>30.402254540112342</v>
       </c>
       <c r="C12" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N12" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="241" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B13" s="213">
         <v>30.945000648638327</v>
       </c>
       <c r="C13" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="241" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B14" s="213">
         <v>31.380791775216256</v>
       </c>
       <c r="C14" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="241" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B15" s="213">
         <v>32.206746329883416</v>
       </c>
       <c r="C15" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N15" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="241" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B16" s="213">
         <v>32.524426366843024</v>
       </c>
       <c r="C16" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="241" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B17" s="213">
         <v>32.981345026600344</v>
       </c>
       <c r="C17" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -37151,81 +37157,81 @@
         <v>34.319028877724222</v>
       </c>
       <c r="C18" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="241" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B19" s="213">
         <v>35.682183173500881</v>
       </c>
       <c r="C19" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="241" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B20" s="213">
         <v>38.661763311151866</v>
       </c>
       <c r="C20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="241" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B21" s="213">
         <v>39.388888631687244</v>
       </c>
       <c r="C21" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="241" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B22" s="213">
         <v>39.74235107400925</v>
       </c>
       <c r="C22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="241" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B23" s="213">
         <v>47.506037136243386</v>
       </c>
       <c r="C23" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F35" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G35" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F36" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G36" s="213">
         <v>22.95063688639036</v>
@@ -37233,10 +37239,10 @@
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F37" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G37" s="213">
         <v>39.852105099621696</v>
@@ -37244,10 +37250,10 @@
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F38" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G38" s="213">
         <v>26.525782164902996</v>
@@ -37255,16 +37261,16 @@
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G39" s="213">
         <v>20.683563775510201</v>
       </c>
       <c r="I39" s="240" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="J39" s="213">
         <v>27.424622059184422</v>
@@ -37272,16 +37278,16 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F40" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G40" s="213">
         <v>37.08791730914588</v>
       </c>
       <c r="I40" s="240" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J40" s="213">
         <v>19.624653880070543</v>
@@ -37289,16 +37295,16 @@
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F41" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G41" s="213">
         <v>23.794487744137435</v>
       </c>
       <c r="I41" s="240" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J41" s="213">
         <v>30.120475709754061</v>
@@ -37306,16 +37312,16 @@
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F42" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G42" s="213">
         <v>45.330450507054664</v>
       </c>
       <c r="I42" s="240" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J42" s="213">
         <v>16.408639172335601</v>
@@ -37323,16 +37329,16 @@
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F43" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G43" s="213">
         <v>51.30722009479716</v>
       </c>
       <c r="I43" s="240" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J43" s="213">
         <v>35.682183173500881</v>
@@ -37340,16 +37346,16 @@
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F44" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G44" s="213">
         <v>47.506037136243386</v>
       </c>
       <c r="I44" s="240" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J44" s="213">
         <v>39.388888631687244</v>
@@ -37357,16 +37363,16 @@
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F45" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G45" s="213">
         <v>35.243378412698405</v>
       </c>
       <c r="I45" s="240" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J45" s="213">
         <v>32.524426366843024</v>
@@ -37374,16 +37380,16 @@
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F46" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G46" s="213">
         <v>32.469379260785509</v>
       </c>
       <c r="I46" s="240" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J46" s="213">
         <v>27.537014329805995</v>
@@ -37391,16 +37397,16 @@
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F47" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G47" s="213">
         <v>43.647444475938528</v>
       </c>
       <c r="I47" s="240" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J47" s="213">
         <v>39.74235107400925</v>
@@ -37408,16 +37414,16 @@
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F48" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G48" s="213">
         <v>35.682183173500881</v>
       </c>
       <c r="I48" s="240" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J48" s="213">
         <v>26.525782164902996</v>
@@ -37425,16 +37431,16 @@
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F49" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G49" s="213">
         <v>39.388888631687244</v>
       </c>
       <c r="I49" s="240" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J49" s="213">
         <v>28.038766469416821</v>
@@ -37442,10 +37448,10 @@
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F50" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G50" s="213">
         <v>42.608970728003136</v>
@@ -37459,16 +37465,16 @@
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F51" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G51" s="213">
         <v>36.013114836860666</v>
       </c>
       <c r="I51" s="240" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J51" s="213">
         <v>30.402254540112342</v>
@@ -37476,7 +37482,7 @@
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F52" t="s">
         <v>429</v>
@@ -37485,7 +37491,7 @@
         <v>42.434777893808594</v>
       </c>
       <c r="I52" s="240" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J52" s="213">
         <v>29.630727402998239</v>
@@ -37493,16 +37499,16 @@
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F53" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G53" s="213">
         <v>36.96287420536207</v>
       </c>
       <c r="I53" s="240" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J53" s="213">
         <v>27.599372894340132</v>
@@ -37510,16 +37516,16 @@
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F54" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G54" s="213">
         <v>35.243128417107584</v>
       </c>
       <c r="I54" s="240" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J54" s="213">
         <v>32.206746329883416</v>
@@ -37527,16 +37533,16 @@
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F55" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G55" s="213">
         <v>28.836014856839725</v>
       </c>
       <c r="I55" s="240" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J55" s="213">
         <v>38.661763311151866</v>
@@ -37544,16 +37550,16 @@
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F56" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G56" s="213">
         <v>36.192417230060741</v>
       </c>
       <c r="I56" s="240" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J56" s="213">
         <v>31.380791775216256</v>
@@ -37561,16 +37567,16 @@
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F57" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G57" s="213">
         <v>30.525970234294224</v>
       </c>
       <c r="I57" s="240" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J57" s="213">
         <v>28.280751212522045</v>
@@ -37578,16 +37584,16 @@
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F58" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G58" s="213">
         <v>35.169445506126429</v>
       </c>
       <c r="I58" s="240" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J58" s="213">
         <v>47.506037136243386</v>
@@ -37595,16 +37601,16 @@
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F59" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G59" s="213">
         <v>37.290314533117765</v>
       </c>
       <c r="I59" s="240" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J59" s="213">
         <v>30.945000648638327</v>
@@ -37612,16 +37618,16 @@
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F60" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G60" s="213">
         <v>41.910624458874452</v>
       </c>
       <c r="I60" s="240" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J60" s="213">
         <v>27.781483718011724</v>
@@ -37629,7 +37635,7 @@
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F61" t="s">
         <v>429</v>
@@ -37638,7 +37644,7 @@
         <v>27.824022254861539</v>
       </c>
       <c r="I61" s="240" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J61" s="213">
         <v>29.02890886648979</v>
@@ -37646,16 +37652,16 @@
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F62" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G62" s="213">
         <v>33.016586361318296</v>
       </c>
       <c r="I62" s="240" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J62" s="213">
         <v>32.981345026600344</v>
@@ -37663,10 +37669,10 @@
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F63" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G63" s="213">
         <v>42.693778260030861</v>
@@ -37674,10 +37680,10 @@
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F64" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G64" s="213">
         <v>38.274715574018956</v>
@@ -37685,10 +37691,10 @@
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F65" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G65" s="213">
         <v>27.632548359158474</v>
@@ -37696,10 +37702,10 @@
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F66" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G66" s="213">
         <v>34.260191207712033</v>
@@ -37707,10 +37713,10 @@
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F67" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G67" s="213">
         <v>28.639971067439323</v>
@@ -37718,10 +37724,10 @@
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F68" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G68" s="213">
         <v>36.095847752700621</v>
@@ -37729,10 +37735,10 @@
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F69" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G69" s="213">
         <v>31.754467120523728</v>
@@ -37740,7 +37746,7 @@
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F70" t="s">
         <v>429</v>
@@ -37751,10 +37757,10 @@
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F71" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G71" s="213">
         <v>20.334016369047614</v>
@@ -37762,10 +37768,10 @@
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F72" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G72" s="213">
         <v>15.867577286470141</v>
@@ -37773,10 +37779,10 @@
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F73" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G73" s="213">
         <v>27.245613219246028</v>
@@ -37784,10 +37790,10 @@
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F74" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G74" s="213">
         <v>18.366437434864515</v>
@@ -37795,10 +37801,10 @@
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F75" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G75" s="213">
         <v>24.481443220899465</v>
@@ -37806,10 +37812,10 @@
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F76" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G76" s="213">
         <v>31.692322987090922</v>
@@ -37817,10 +37823,10 @@
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F77" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G77" s="213">
         <v>32.524426366843024</v>
@@ -37828,10 +37834,10 @@
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F78" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G78" s="213">
         <v>42.00342585243974</v>
@@ -37839,7 +37845,7 @@
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F79" t="s">
         <v>429</v>
@@ -37850,10 +37856,10 @@
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
+        <v>660</v>
+      </c>
+      <c r="F80" t="s">
         <v>661</v>
-      </c>
-      <c r="F80" t="s">
-        <v>662</v>
       </c>
       <c r="G80" s="213">
         <v>28.380749448853617</v>
@@ -37861,10 +37867,10 @@
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F81" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G81" s="213">
         <v>25.63246458700764</v>
@@ -37872,10 +37878,10 @@
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F82" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G82" s="213">
         <v>55.50145167670977</v>
@@ -37883,10 +37889,10 @@
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F83" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G83" s="213">
         <v>27.198181020093219</v>
@@ -37894,10 +37900,10 @@
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F84" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G84" s="213">
         <v>31.173061311973349</v>
@@ -37905,10 +37911,10 @@
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F85" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G85" s="213">
         <v>26.381201381540269</v>
@@ -37916,10 +37922,10 @@
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F86" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G86" s="213">
         <v>25.353459091159618</v>
@@ -37927,10 +37933,10 @@
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F87" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G87" s="213">
         <v>30.289309537588181</v>
@@ -37938,10 +37944,10 @@
     </row>
     <row r="88" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F88" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G88" s="213">
         <v>23.365360931553415</v>
@@ -37949,10 +37955,10 @@
     </row>
     <row r="89" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F89" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G89" s="213">
         <v>34.106273467813054</v>
@@ -37960,10 +37966,10 @@
     </row>
     <row r="90" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F90" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G90" s="213">
         <v>30.148575412572431</v>
@@ -37971,10 +37977,10 @@
     </row>
     <row r="91" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F91" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G91" s="213">
         <v>30.880705357142858</v>
@@ -37982,10 +37988,10 @@
     </row>
     <row r="92" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F92" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G92" s="213">
         <v>15.70180640064668</v>
@@ -37993,10 +37999,10 @@
     </row>
     <row r="93" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F93" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G93" s="213">
         <v>29.446578865110858</v>
@@ -38004,10 +38010,10 @@
     </row>
     <row r="94" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F94" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G94" s="213">
         <v>30.222234827727384</v>
@@ -38015,10 +38021,10 @@
     </row>
     <row r="95" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F95" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G95" s="213">
         <v>38.18638007842025</v>
@@ -38026,10 +38032,10 @@
     </row>
     <row r="96" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E96" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F96" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G96" s="213">
         <v>27.795863931143444</v>
@@ -38037,10 +38043,10 @@
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F97" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G97" s="213">
         <v>25.135419781955989</v>
@@ -38048,10 +38054,10 @@
     </row>
     <row r="98" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F98" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G98" s="213">
         <v>25.693865019240015</v>
@@ -38059,10 +38065,10 @@
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F99" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G99" s="213">
         <v>22.232704472803427</v>
@@ -38070,10 +38076,10 @@
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
+        <v>664</v>
+      </c>
+      <c r="F100" t="s">
         <v>665</v>
-      </c>
-      <c r="F100" t="s">
-        <v>666</v>
       </c>
       <c r="G100" s="213">
         <v>19.624653880070543</v>
@@ -38081,10 +38087,10 @@
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F101" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G101" s="213">
         <v>16.408639172335601</v>
@@ -38092,10 +38098,10 @@
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F102" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G102" s="213">
         <v>27.537014329805995</v>
@@ -38103,10 +38109,10 @@
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F103" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G103" s="213">
         <v>35.422500253527332</v>
@@ -38114,10 +38120,10 @@
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F104" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G104" s="213">
         <v>31.455214455297785</v>
@@ -38125,10 +38131,10 @@
     </row>
     <row r="105" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F105" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G105" s="213">
         <v>29.3269381180713</v>
@@ -38136,10 +38142,10 @@
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F106" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G106" s="213">
         <v>31.383404824368014</v>
@@ -38147,10 +38153,10 @@
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F107" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G107" s="213">
         <v>27.287852057613165</v>
@@ -38158,10 +38164,10 @@
     </row>
     <row r="108" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E108" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F108" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G108" s="213">
         <v>28.280751212522045</v>
@@ -38169,10 +38175,10 @@
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F109" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G109" s="213">
         <v>31.193894277875756</v>
@@ -38180,10 +38186,10 @@
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F110" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G110" s="213">
         <v>29.560536333265496</v>
@@ -38191,10 +38197,10 @@
     </row>
     <row r="111" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E111" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F111" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G111" s="213">
         <v>34.451178099017383</v>
@@ -38202,10 +38208,10 @@
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E112" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F112" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G112" s="213">
         <v>26.992157868008317</v>
@@ -38213,10 +38219,10 @@
     </row>
     <row r="113" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E113" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F113" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G113" s="213">
         <v>28.078254783950612</v>
@@ -38224,10 +38230,10 @@
     </row>
     <row r="114" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E114" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F114" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G114" s="213">
         <v>42.292557657785338</v>
@@ -38235,10 +38241,10 @@
     </row>
     <row r="115" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F115" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G115" s="213">
         <v>21.893363866843032</v>
@@ -38246,7 +38252,7 @@
     </row>
     <row r="116" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F116" t="s">
         <v>429</v>
@@ -38257,10 +38263,10 @@
     </row>
     <row r="117" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E117" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F117" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G117" s="213">
         <v>24.609878455687827</v>
@@ -38268,10 +38274,10 @@
     </row>
     <row r="118" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E118" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F118" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G118" s="213">
         <v>28.207419172545556</v>
@@ -38279,10 +38285,10 @@
     </row>
     <row r="119" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E119" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F119" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G119" s="213">
         <v>31.297299572172616</v>
@@ -38290,10 +38296,10 @@
     </row>
     <row r="120" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E120" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F120" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G120" s="213">
         <v>37.92700965293524</v>
@@ -38301,10 +38307,10 @@
     </row>
     <row r="121" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E121" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F121" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G121" s="213">
         <v>28.049114672894618</v>
@@ -38312,10 +38318,10 @@
     </row>
     <row r="122" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E122" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F122" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G122" s="213">
         <v>21.913738507495587</v>
@@ -38323,10 +38329,10 @@
     </row>
     <row r="123" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E123" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F123" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G123" s="213">
         <v>31.17445017636684</v>

</xml_diff>